<commit_message>
Minor changes after merge issues
</commit_message>
<xml_diff>
--- a/assignment_4/rat_data.xlsx
+++ b/assignment_4/rat_data.xlsx
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:H51" si="0">IF(AND(B2&lt;D2,C2=0),1,0)</f>
+        <f t="shared" ref="G2:G51" si="0">IF(AND(B2&lt;D2,C2=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="H2">

</xml_diff>